<commit_message>
fix: SINAPI price enrichment + show 'Sem Preço' when unavailable
</commit_message>
<xml_diff>
--- a/tmp/sintetico-gerado.xlsx
+++ b/tmp/sintetico-gerado.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="45">
   <si>
     <t>MOCK CO</t>
   </si>
@@ -19,63 +19,69 @@
     <t>CNPJ: 00.000.000/0000-00</t>
   </si>
   <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Responsável Técnico: Mock Eng | CREA/CAU: 000.000-0 | CPF: 000.000.000-00 | Contato: mock@example.com | (11) 99999-9999</t>
+  </si>
+  <si>
+    <t>ORÇAMENTO SINTÉTICO</t>
+  </si>
+  <si>
+    <t>OBRA: MOCK BUDGET</t>
+  </si>
+  <si>
+    <t>CLIENTE: CLIENT MOCK</t>
+  </si>
+  <si>
+    <t>DATA: 21/01/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BASES DE REFERÊNCIA: SINAPI (01/2025/SP) </t>
+  </si>
+  <si>
+    <t>BDI: NÃO DESONERADO - 20.00%</t>
+  </si>
+  <si>
+    <t>ENCARGOS SOCIAIS: Horista 85.00% | Mensalista 85.00%</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Banco</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Und</t>
+  </si>
+  <si>
+    <t>Quant.</t>
+  </si>
+  <si>
+    <t>Valor Unit</t>
+  </si>
+  <si>
+    <t>Valor Unit com BDI</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Peso (%)</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>ORÇAMENTO SINTÉTICO</t>
-  </si>
-  <si>
-    <t>OBRA: MOCK BUDGET</t>
-  </si>
-  <si>
-    <t>CLIENTE: CLIENT MOCK</t>
-  </si>
-  <si>
-    <t>DATA: 20/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BASES DE REFERÊNCIA: SINAPI (01/2025/SP) </t>
-  </si>
-  <si>
-    <t>BDI: NÃO DESONERADO - 20.00%</t>
-  </si>
-  <si>
-    <t>ENCARGOS SOCIAIS: Horista 85.00% | Mensalista 85.00%</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Código</t>
-  </si>
-  <si>
-    <t>Banco</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Und</t>
-  </si>
-  <si>
-    <t>Quant.</t>
-  </si>
-  <si>
-    <t>Valor Unit</t>
-  </si>
-  <si>
-    <t>Valor Unit com BDI</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Peso (%)</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Group 1</t>
   </si>
   <si>
@@ -139,7 +145,7 @@
     <t>CREA/CAU / CPF NÃO INFORMADO</t>
   </si>
   <si>
-    <t>Emitido em: 20/01/2026 às 23:52:23</t>
+    <t>Emitido em: 21/01/2026 às 00:11:39</t>
   </si>
 </sst>
 </file>
@@ -149,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$ &quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -166,6 +172,11 @@
       <sz val="10"/>
     </font>
     <font>
+      <color rgb="FF666666"/>
+      <sz val="9"/>
+    </font>
+    <font>
+      <i/>
       <color rgb="FF666666"/>
       <sz val="9"/>
     </font>
@@ -280,35 +291,37 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -341,10 +354,6 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -354,12 +363,16 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -704,7 +717,7 @@
   <dimension ref="A1:J31"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="10" width="54" customWidth="1"/>
+    <col min="1" max="10" width="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -749,161 +762,176 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
     <row r="5" ht="25" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="A11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="A12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="A13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="16" ht="22" customHeight="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="D16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="E16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="F16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="G16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="H16" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="I16" s="11" t="s">
         <v>19</v>
       </c>
+      <c r="J16" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="A17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="13">
+      <c r="B17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="14">
         <v>1</v>
       </c>
-      <c r="G17" s="14"/>
+      <c r="G17" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="H17" s="15">
         <v>2000</v>
       </c>
@@ -916,19 +944,19 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F18" s="19">
         <v>10</v>
@@ -948,19 +976,19 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F19" s="24">
         <v>5</v>
@@ -979,25 +1007,27 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="13">
+      <c r="A20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="14">
         <v>1</v>
       </c>
-      <c r="G20" s="14"/>
+      <c r="G20" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="H20" s="15">
         <v>500</v>
       </c>
@@ -1010,19 +1040,19 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F21" s="24">
         <v>50</v>
@@ -1043,7 +1073,7 @@
     <row r="22" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F23" s="27" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H23" s="28">
         <v>2500</v>
@@ -1051,7 +1081,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F24" s="29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H24" s="30">
         <v>0</v>
@@ -1059,7 +1089,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F25" s="31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H25" s="32">
         <v>2500</v>
@@ -1069,7 +1099,7 @@
     <row r="27" spans="1:10" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
@@ -1083,7 +1113,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
@@ -1097,7 +1127,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B30" s="34"/>
       <c r="C30" s="34"/>
@@ -1111,7 +1141,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B31" s="35"/>
       <c r="C31" s="35"/>
@@ -1124,10 +1154,11 @@
       <c r="J31" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A7:J7"/>
     <mergeCell ref="A8:J8"/>

</xml_diff>